<commit_message>
Fixed the slab suction calculation; it is rejected by the inversion after all....
</commit_message>
<xml_diff>
--- a/notebooks/settings.xlsx
+++ b/notebooks/settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Documents/_Plato/Plato/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA88DCC-682D-2C4E-97F9-E5EF0AA51942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BED031B-5784-6A4C-B57F-AC24DD04067E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="2" xr2:uid="{745898CB-6A96-6A42-A7F0-C6C371FC8CE9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -283,13 +283,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,7 +628,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="A1:XFD1048576"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1039,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F237874-3774-8A44-880A-D4D01C91DA6A}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1051,14 +1052,15 @@
     <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1072,22 +1074,19 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
-      </c>
-      <c r="G1" t="s">
-        <v>21</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1100,23 +1099,21 @@
       <c r="D2" t="b">
         <v>0</v>
       </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>150000</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
+      <c r="E2" s="2">
+        <v>1.7E+20</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>150000</v>
       </c>
       <c r="H2" s="1">
-        <v>5.6899999999999999E-2</v>
-      </c>
-      <c r="I2">
-        <v>1.64E+20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>5.8099999999999999E-2</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1129,23 +1126,21 @@
       <c r="D3" t="b">
         <v>0</v>
       </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>150000</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
+      <c r="E3" s="2">
+        <v>1.7E+20</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>150000</v>
       </c>
       <c r="H3" s="1">
-        <v>5.6899999999999999E-2</v>
-      </c>
-      <c r="I3">
-        <v>1.64E+20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>5.8099999999999999E-2</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1158,23 +1153,21 @@
       <c r="D4" t="b">
         <v>1</v>
       </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>150000</v>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
+      <c r="E4" s="2">
+        <v>1.7E+20</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>150000</v>
       </c>
       <c r="H4" s="1">
-        <v>5.6899999999999999E-2</v>
-      </c>
-      <c r="I4">
-        <v>1.64E+20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>5.8099999999999999E-2</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1187,23 +1180,21 @@
       <c r="D5" t="b">
         <v>0</v>
       </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>150000</v>
-      </c>
-      <c r="G5" t="b">
-        <v>0</v>
+      <c r="E5" s="2">
+        <v>1.7E+20</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>150000</v>
       </c>
       <c r="H5" s="1">
-        <v>5.6899999999999999E-2</v>
-      </c>
-      <c r="I5">
-        <v>1.64E+20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>5.8099999999999999E-2</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1216,21 +1207,19 @@
       <c r="D6" t="b">
         <v>1</v>
       </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
-        <v>150000</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
+      <c r="E6" s="2">
+        <v>1.7E+20</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>150000</v>
       </c>
       <c r="H6" s="1">
-        <v>5.6899999999999999E-2</v>
-      </c>
-      <c r="I6">
-        <v>1.64E+20</v>
-      </c>
+        <v>5.8099999999999999E-2</v>
+      </c>
+      <c r="J6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1239,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD252801-88B0-B74D-8EF9-ED356E964EDA}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1254,11 +1243,13 @@
     <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1280,14 +1271,20 @@
       <c r="G1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1307,16 +1304,22 @@
         <v>2000</v>
       </c>
       <c r="G2" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H2" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I2" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J2" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K2" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
@@ -1336,16 +1339,22 @@
         <v>2000</v>
       </c>
       <c r="G3" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H3" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I3" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J3" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K3" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -1365,16 +1374,22 @@
         <v>2000</v>
       </c>
       <c r="G4" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H4" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I4" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J4" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K4" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>42</v>
       </c>
@@ -1394,16 +1409,22 @@
         <v>2000</v>
       </c>
       <c r="G5" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H5" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I5" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J5" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K5" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>44</v>
       </c>
@@ -1423,16 +1444,22 @@
         <v>2000</v>
       </c>
       <c r="G6" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H6" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I6" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J6" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K6" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
@@ -1452,16 +1479,22 @@
         <v>2000</v>
       </c>
       <c r="G7" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H7" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I7" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J7" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K7" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>46</v>
       </c>
@@ -1481,16 +1514,22 @@
         <v>2000</v>
       </c>
       <c r="G8" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H8" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I8" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J8" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K8" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>47</v>
       </c>
@@ -1510,16 +1549,22 @@
         <v>2000</v>
       </c>
       <c r="G9" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H9" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I9" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J9" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K9" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>48</v>
       </c>
@@ -1539,16 +1584,22 @@
         <v>2000</v>
       </c>
       <c r="G10" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H10" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I10" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J10" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K10" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>49</v>
       </c>
@@ -1568,16 +1619,22 @@
         <v>2000</v>
       </c>
       <c r="G11" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H11" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I11" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J11" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K11" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>50</v>
       </c>
@@ -1597,16 +1654,22 @@
         <v>2000</v>
       </c>
       <c r="G12" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H12" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I12" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J12" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K12" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>51</v>
       </c>
@@ -1626,16 +1689,22 @@
         <v>2000</v>
       </c>
       <c r="G13" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H13" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I13" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J13" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K13" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>52</v>
       </c>
@@ -1655,16 +1724,22 @@
         <v>2000</v>
       </c>
       <c r="G14" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H14" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I14" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J14" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K14" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>54</v>
       </c>
@@ -1684,16 +1759,22 @@
         <v>2000</v>
       </c>
       <c r="G15" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H15" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I15" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J15" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K15" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>56</v>
       </c>
@@ -1713,16 +1794,22 @@
         <v>1000</v>
       </c>
       <c r="G16" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H16" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I16" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J16" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K16" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>57</v>
       </c>
@@ -1742,16 +1829,22 @@
         <v>500</v>
       </c>
       <c r="G17" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H17" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I17" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J17" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K17" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>58</v>
       </c>
@@ -1771,16 +1864,22 @@
         <v>100</v>
       </c>
       <c r="G18" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H18" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I18" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J18" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K18" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>59</v>
       </c>
@@ -1800,16 +1899,22 @@
         <v>500</v>
       </c>
       <c r="G19" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H19" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I19" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J19" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K19" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>61</v>
       </c>
@@ -1829,16 +1934,22 @@
         <v>500</v>
       </c>
       <c r="G20" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H20" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I20" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J20" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K20" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>65</v>
       </c>
@@ -1858,16 +1969,22 @@
         <v>2000</v>
       </c>
       <c r="G21" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H21" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I21" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J21" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K21" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>63</v>
       </c>
@@ -1887,16 +2004,22 @@
         <v>100</v>
       </c>
       <c r="G22" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H22" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I22" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J22" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K22" s="4">
         <v>7500000000000</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>64</v>
       </c>
@@ -1916,12 +2039,18 @@
         <v>100</v>
       </c>
       <c r="G23" s="4">
-        <v>1.22E+20</v>
-      </c>
-      <c r="H23" s="3">
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="I23" s="4">
+        <v>1.7E+20</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J23" s="6">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="K23" s="4">
         <v>7500000000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
small updates to notebook 2b
</commit_message>
<xml_diff>
--- a/notebooks/settings.xlsx
+++ b/notebooks/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Documents/_Plato/Plato/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF00F6B-02A6-3240-9B3B-8C5F3AB0BC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650801BD-993E-0F4B-8768-5A6215965C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="2" xr2:uid="{745898CB-6A96-6A42-A7F0-C6C371FC8CE9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{745898CB-6A96-6A42-A7F0-C6C371FC8CE9}"/>
   </bookViews>
   <sheets>
     <sheet name="2a - Extended torque balance" sheetId="4" r:id="rId1"/>
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F237874-3774-8A44-880A-D4D01C91DA6A}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1023,7 +1023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD252801-88B0-B74D-8EF9-ED356E964EDA}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated a bunch of stuff
</commit_message>
<xml_diff>
--- a/notebooks/settings.xlsx
+++ b/notebooks/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Documents/_Plato/Plato/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650801BD-993E-0F4B-8768-5A6215965C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B4AAE2-A80B-E644-A717-6DA497C8BE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{745898CB-6A96-6A42-A7F0-C6C371FC8CE9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="4" xr2:uid="{745898CB-6A96-6A42-A7F0-C6C371FC8CE9}"/>
   </bookViews>
   <sheets>
     <sheet name="2a - Extended torque balance" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -835,7 +835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F237874-3774-8A44-880A-D4D01C91DA6A}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -1714,32 +1714,47 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8233F98-E437-7E49-BB85-51A85E23E447}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1749,27 +1764,39 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1104F42-BC22-3042-AC9B-E2E6D371AD2B}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>